<commit_message>
Retoco enlace a js de premium
</commit_message>
<xml_diff>
--- a/Calendario de equipo.xlsx
+++ b/Calendario de equipo.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Desktop\Proyecto Pochadia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Desktop\Proyecto pochadia GIT\Proyecto-Pochadia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCDFA11-C599-4679-AA01-733E26D700B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305015B3-1C7D-4059-ABF6-90861FAC2CB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2163E87C-8AB4-41C6-BF70-95D389878E2E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{2163E87C-8AB4-41C6-BF70-95D389878E2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Manuel</t>
   </si>
@@ -82,13 +82,25 @@
   </si>
   <si>
     <t xml:space="preserve">Organizar un repositorio de GIT para el proyecto y comenzar a utilizarlo. Crear los casos de uso. Comenzar el modelado de la base de datos y sus requerimientos del sistema así como la instalación y configuración de MySQL </t>
+  </si>
+  <si>
+    <t>3h</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>Tutorias</t>
+  </si>
+  <si>
+    <t>Siguiente turoría día 12 16:00h</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,13 +116,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -125,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -141,6 +167,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -493,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B68DF2F6-E898-459B-BA00-DF9104F8D6AF}">
-  <dimension ref="A5:G11"/>
+  <dimension ref="A5:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,6 +605,61 @@
         <v>14</v>
       </c>
     </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="6">
+        <v>43987</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="6">
+        <v>43994</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="6">
+        <v>44014</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="6">
+        <v>44031</v>
+      </c>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="6">
+        <v>44046</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="6">
+        <v>44053</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualizo el calendario de equipo
</commit_message>
<xml_diff>
--- a/Calendario de equipo.xlsx
+++ b/Calendario de equipo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Desktop\Proyecto pochadia GIT\Proyecto-Pochadia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305015B3-1C7D-4059-ABF6-90861FAC2CB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD861D0-82DF-4E35-A647-963A97E55B07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{2163E87C-8AB4-41C6-BF70-95D389878E2E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Manuel</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Tareas grupales</t>
   </si>
   <si>
-    <t>Buscar información acerca de si es posible realizar un stream de videojuegos con Java. Tarea de investigación, hay que tener una respuesta el día 29.</t>
-  </si>
-  <si>
     <t>Semana 25-29/05</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t>Comenzar con el powerPoint de presentación del proyecto. Comenzar tareas de investigación del frontend y comenzando plantillas HTML/CSS de las distintas pantallas.</t>
   </si>
   <si>
-    <t>Realizar los prototipos de las pantallas. Realizar el esquema de navegación de pantallas. Realizar el diagrama de secuencia.</t>
-  </si>
-  <si>
     <t>Terminar la realización de los prototipos. Montar un servidor para estimar la cantidad de jugadores que se pueden tener en un mismo servidor y intentar conexiones cliente/servidor.</t>
   </si>
   <si>
@@ -93,14 +87,60 @@
     <t>Tutorias</t>
   </si>
   <si>
-    <t>Siguiente turoría día 12 16:00h</t>
+    <t>Comenzar front con páginas que le tocan.</t>
+  </si>
+  <si>
+    <t>Comenzar con los esquemas de la base de datos de entidad relación y hacer datos de prueba para una primera carga. Realizar los diferentes esquemas requeridos.</t>
+  </si>
+  <si>
+    <t>Continuar con páginas del front que le tocan, probar implementación de json con angular.</t>
+  </si>
+  <si>
+    <t>Continuar con páginas que le tocan, probar implementación del json con angular.</t>
+  </si>
+  <si>
+    <t>Hacer front con páginas que le tocan. Probar integración de json en las pág con angular, retocar la BBDD.</t>
+  </si>
+  <si>
+    <t>Continuar retocando front y perfilando. Realizar json de get y post de las páginas que le tocan.</t>
+  </si>
+  <si>
+    <t>Continuar retocando front y perfilando. Realizar json de get y post de las páginas que le tocan. Retocar BBDD, Investigar si es necesario vistas, procedimientos, disparadores, acciones etc..</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Buscar información acerca de si es posible realizar un stream de videojuegos con Java. Tarea de investigación, hay que tener una respuesta el día 29. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SE PUEDE</t>
+    </r>
+  </si>
+  <si>
+    <t>Json de las diferentes páginas, averiguar como funciona bien angular para poder hacer nuestras páginas dinamicas.</t>
+  </si>
+  <si>
+    <t>Siguiente turoría día 18 16:00h</t>
+  </si>
+  <si>
+    <t>0,5h</t>
+  </si>
+  <si>
+    <t>Horas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,8 +164,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,6 +183,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -151,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -168,10 +228,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,7 +598,7 @@
   <dimension ref="A5:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,25 +616,25 @@
   <sheetData>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>10</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -570,7 +642,16 @@
         <v>0</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -578,7 +659,16 @@
         <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -586,7 +676,16 @@
         <v>1</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -594,71 +693,75 @@
         <v>3</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>20</v>
+      <c r="B15" s="11" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
-        <v>19</v>
+      <c r="B17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="6">
+      <c r="B18" s="9">
         <v>43987</v>
       </c>
-      <c r="C18" t="s">
-        <v>17</v>
+      <c r="C18" s="10" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="6">
+      <c r="B19" s="9">
         <v>43994</v>
       </c>
-      <c r="C19" t="s">
-        <v>17</v>
+      <c r="C19" s="10" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="6">
+      <c r="B20" s="9">
         <v>44014</v>
       </c>
-      <c r="C20" t="s">
-        <v>18</v>
+      <c r="C20" s="10" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="6">
-        <v>44031</v>
-      </c>
-      <c r="C21" t="s">
-        <v>18</v>
+      <c r="B21" s="8">
+        <v>44030</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="6">
+      <c r="B22" s="8">
         <v>44046</v>
       </c>
-      <c r="C22" t="s">
-        <v>18</v>
+      <c r="C22" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="6">
+      <c r="B23" s="8">
         <v>44053</v>
       </c>
+      <c r="C23" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>